<commit_message>
All testing approach done
</commit_message>
<xml_diff>
--- a/Time_required.xlsx
+++ b/Time_required.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\hospital-management-software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AB3F9E-A893-4E51-A5C0-4342556939E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8701306F-D70D-4C87-BC78-CEAB67E41771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Serial No.</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>17-04-2022</t>
+  </si>
+  <si>
+    <t>3 hours 20 minitues + seheri + other</t>
+  </si>
+  <si>
+    <t>Black Box Testing Done</t>
   </si>
 </sst>
 </file>
@@ -434,7 +440,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,17 +483,29 @@
       <c r="C2" s="7">
         <v>9.0277777777777776E-2</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="D2" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.9375</v>
+      </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
@@ -495,9 +513,15 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2.9166666666666664E-2</v>
+      </c>
+      <c r="D4" s="6">
+        <v>4.6527777777777779E-2</v>
+      </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>

</xml_diff>